<commit_message>
Manage Interviewers - Bug Fixes
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -1117,7 +1117,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1364,7 +1364,7 @@
           <t>2021-06-16</t>
         </is>
       </c>
-      <c r="B9" s="10" t="n">
+      <c r="B9" s="8" t="n">
         <v>44363.68051387731</v>
       </c>
       <c r="C9" s="5" t="inlineStr">
@@ -1386,39 +1386,85 @@
       </c>
     </row>
     <row r="10" ht="13.8" customHeight="1" s="6">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="5" t="inlineStr">
         <is>
           <t>2021-06-16</t>
         </is>
       </c>
-      <c r="B10" s="10" t="n">
-        <v>44363.78083806514</v>
-      </c>
-      <c r="C10" t="inlineStr">
+      <c r="B10" s="8" t="n">
+        <v>44363.78083806713</v>
+      </c>
+      <c r="C10" s="5" t="inlineStr">
         <is>
           <t>live_145_hf2</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>269</v>
-      </c>
-      <c r="E10" t="n">
+      <c r="D10" s="5" t="n">
+        <v>269</v>
+      </c>
+      <c r="E10" s="5" t="n">
         <v>266</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10" s="5" t="n">
         <v>3</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10" s="5" t="n">
         <v>4.24</v>
       </c>
     </row>
     <row r="11" ht="15" customHeight="1" s="6">
-      <c r="B11" s="8" t="n"/>
-      <c r="D11" s="9" t="n"/>
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>2021-06-17</t>
+        </is>
+      </c>
+      <c r="B11" s="8" t="n">
+        <v>44364.54191730324</v>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
+        <is>
+          <t>145_data_hstry</t>
+        </is>
+      </c>
+      <c r="D11" s="9" t="n">
+        <v>269</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>267</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="5" t="n">
+        <v>4.28</v>
+      </c>
     </row>
     <row r="12" ht="15" customHeight="1" s="6">
-      <c r="B12" s="8" t="n"/>
-      <c r="D12" s="9" t="n"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2021-06-17</t>
+        </is>
+      </c>
+      <c r="B12" s="10" t="n">
+        <v>44364.58163298016</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>145_hstry_data</t>
+        </is>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>269</v>
+      </c>
+      <c r="E12" t="n">
+        <v>268</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>4.11</v>
+      </c>
     </row>
     <row r="13" ht="15" customHeight="1" s="6">
       <c r="B13" s="8" t="n"/>

</xml_diff>

<commit_message>
Mass Interview uncheck for Only Available Interviewers
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -19,9 +19,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -492,13 +493,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.17" customWidth="1" style="6" min="1" max="1"/>
     <col width="19.44" customWidth="1" style="6" min="2" max="2"/>
@@ -1250,12 +1251,86 @@
       </c>
     </row>
     <row r="28" ht="13.8" customHeight="1" s="7">
-      <c r="B28" s="9" t="n"/>
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>2021-10-26</t>
+        </is>
+      </c>
+      <c r="B28" s="11" t="n">
+        <v>44495.64163151621</v>
+      </c>
+      <c r="C28" s="6" t="inlineStr">
+        <is>
+          <t>152_fstcycle</t>
+        </is>
+      </c>
+      <c r="D28" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E28" s="6" t="n">
+        <v>263</v>
+      </c>
+      <c r="F28" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="G28" s="6" t="n">
+        <v>6.52</v>
+      </c>
     </row>
     <row r="29" ht="13.8" customHeight="1" s="7">
-      <c r="B29" s="9" t="n"/>
-    </row>
-    <row r="30" ht="13.8" customHeight="1" s="7"/>
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>2021-10-27</t>
+        </is>
+      </c>
+      <c r="B29" s="11" t="n">
+        <v>44496.64047292824</v>
+      </c>
+      <c r="C29" s="6" t="inlineStr">
+        <is>
+          <t>152_scndcycle</t>
+        </is>
+      </c>
+      <c r="D29" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E29" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F29" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" s="6" t="n">
+        <v>6.88</v>
+      </c>
+    </row>
+    <row r="30" ht="13.8" customHeight="1" s="7">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>2021-10-28</t>
+        </is>
+      </c>
+      <c r="B30" s="12" t="n">
+        <v>44497.38131106481</v>
+      </c>
+      <c r="C30" s="6" t="inlineStr">
+        <is>
+          <t>152_fnlrgrsn</t>
+        </is>
+      </c>
+      <c r="D30" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E30" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F30" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" s="6" t="n">
+        <v>5.8</v>
+      </c>
+    </row>
     <row r="31" ht="13.8" customHeight="1" s="7"/>
     <row r="32" ht="13.8" customHeight="1" s="7"/>
     <row r="33" ht="13.8" customHeight="1" s="7"/>
@@ -1283,7 +1358,7 @@
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.17" customWidth="1" style="6" min="1" max="1"/>
     <col width="19.44" customWidth="1" style="6" min="2" max="2"/>
@@ -1684,11 +1759,58 @@
       </c>
     </row>
     <row r="15" ht="15" customHeight="1" s="7">
-      <c r="B15" s="9" t="n"/>
-      <c r="D15" s="10" t="n"/>
+      <c r="A15" s="6" t="inlineStr">
+        <is>
+          <t>2021-10-28</t>
+        </is>
+      </c>
+      <c r="B15" s="11" t="n">
+        <v>44497.61923534722</v>
+      </c>
+      <c r="C15" s="6" t="inlineStr">
+        <is>
+          <t>152_beta</t>
+        </is>
+      </c>
+      <c r="D15" s="10" t="n">
+        <v>269</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F15" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <v>5.35</v>
+      </c>
     </row>
     <row r="16" ht="15" customHeight="1" s="7">
-      <c r="B16" s="9" t="n"/>
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>2021-10-28</t>
+        </is>
+      </c>
+      <c r="B16" s="11" t="n">
+        <v>44497.69705530092</v>
+      </c>
+      <c r="C16" s="6" t="inlineStr">
+        <is>
+          <t>152_betachgs</t>
+        </is>
+      </c>
+      <c r="D16" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <v>266</v>
+      </c>
+      <c r="F16" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>5.28</v>
+      </c>
     </row>
     <row r="1048576" ht="15" customHeight="1" s="7"/>
   </sheetData>
@@ -1704,13 +1826,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.17" customWidth="1" style="6" min="1" max="1"/>
     <col width="19.44" customWidth="1" style="6" min="2" max="2"/>
@@ -2513,6 +2635,33 @@
       </c>
       <c r="G29" s="6" t="n">
         <v>6.08</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2021-10-28</t>
+        </is>
+      </c>
+      <c r="B30" s="12" t="n">
+        <v>44497.85545837627</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>152_livetest</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>269</v>
+      </c>
+      <c r="E30" t="n">
+        <v>268</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G30" t="n">
+        <v>4.63</v>
       </c>
     </row>
   </sheetData>
@@ -2534,7 +2683,7 @@
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col width="11.17" customWidth="1" style="6" min="1" max="1"/>
     <col width="19.44" customWidth="1" style="6" min="2" max="2"/>

</xml_diff>

<commit_message>
fixes in HTML report
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
@@ -1331,11 +1331,573 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="31" ht="13.8" customHeight="1" s="7"/>
-    <row r="32" ht="13.8" customHeight="1" s="7"/>
-    <row r="33" ht="13.8" customHeight="1" s="7"/>
-    <row r="34" ht="13.8" customHeight="1" s="7"/>
-    <row r="35" ht="13.8" customHeight="1" s="7"/>
+    <row r="31" ht="13.8" customHeight="1" s="7">
+      <c r="A31" s="6" t="inlineStr">
+        <is>
+          <t>2021-11-17</t>
+        </is>
+      </c>
+      <c r="B31" s="12" t="n">
+        <v>44517.6023143287</v>
+      </c>
+      <c r="C31" s="6" t="inlineStr">
+        <is>
+          <t>153rsgn</t>
+        </is>
+      </c>
+      <c r="D31" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E31" s="6" t="n">
+        <v>265</v>
+      </c>
+      <c r="F31" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G31" s="6" t="n">
+        <v>6.82</v>
+      </c>
+    </row>
+    <row r="32" ht="13.8" customHeight="1" s="7">
+      <c r="A32" s="6" t="inlineStr">
+        <is>
+          <t>2021-11-18</t>
+        </is>
+      </c>
+      <c r="B32" s="12" t="n">
+        <v>44518.42095861111</v>
+      </c>
+      <c r="C32" s="6" t="inlineStr">
+        <is>
+          <t>153fnlrgsn</t>
+        </is>
+      </c>
+      <c r="D32" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E32" s="6" t="n">
+        <v>259</v>
+      </c>
+      <c r="F32" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G32" s="6" t="n">
+        <v>8.960000000000001</v>
+      </c>
+    </row>
+    <row r="33" ht="13.8" customHeight="1" s="7">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>2021-11-29</t>
+        </is>
+      </c>
+      <c r="B33" s="12" t="n">
+        <v>44529.74459321759</v>
+      </c>
+      <c r="C33" s="6" t="inlineStr">
+        <is>
+          <t>153_htfix</t>
+        </is>
+      </c>
+      <c r="D33" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E33" s="6" t="n">
+        <v>263</v>
+      </c>
+      <c r="F33" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="G33" s="6" t="n">
+        <v>8.01</v>
+      </c>
+    </row>
+    <row r="34" ht="13.8" customHeight="1" s="7">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t>2021-12-03</t>
+        </is>
+      </c>
+      <c r="B34" s="12" t="n">
+        <v>44533.71769680556</v>
+      </c>
+      <c r="C34" s="6" t="inlineStr">
+        <is>
+          <t>154_scndrgsn</t>
+        </is>
+      </c>
+      <c r="D34" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E34" s="6" t="n">
+        <v>261</v>
+      </c>
+      <c r="F34" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="G34" s="6" t="n">
+        <v>6.84</v>
+      </c>
+    </row>
+    <row r="35" ht="13.8" customHeight="1" s="7">
+      <c r="A35" s="6" t="inlineStr">
+        <is>
+          <t>2021-12-06</t>
+        </is>
+      </c>
+      <c r="B35" s="12" t="n">
+        <v>44536.4428</v>
+      </c>
+      <c r="C35" s="6" t="inlineStr">
+        <is>
+          <t>154_fnlrgsn</t>
+        </is>
+      </c>
+      <c r="D35" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E35" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F35" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G35" s="6" t="n">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="inlineStr">
+        <is>
+          <t>2021-12-22</t>
+        </is>
+      </c>
+      <c r="B36" s="12" t="n">
+        <v>44552.41040861111</v>
+      </c>
+      <c r="C36" s="6" t="inlineStr">
+        <is>
+          <t>sprint155</t>
+        </is>
+      </c>
+      <c r="D36" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E36" s="6" t="n">
+        <v>266</v>
+      </c>
+      <c r="F36" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G36" s="6" t="n">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>2022-01-03</t>
+        </is>
+      </c>
+      <c r="B37" s="12" t="n">
+        <v>44564.62398364583</v>
+      </c>
+      <c r="C37" s="6" t="inlineStr">
+        <is>
+          <t>lodash</t>
+        </is>
+      </c>
+      <c r="D37" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E37" s="6" t="n">
+        <v>248</v>
+      </c>
+      <c r="F37" s="6" t="n">
+        <v>21</v>
+      </c>
+      <c r="G37" s="6" t="n">
+        <v>10.39</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="inlineStr">
+        <is>
+          <t>2022-01-17</t>
+        </is>
+      </c>
+      <c r="B38" s="12" t="n">
+        <v>44578.52386765046</v>
+      </c>
+      <c r="C38" s="6" t="inlineStr">
+        <is>
+          <t>frstrgsn156</t>
+        </is>
+      </c>
+      <c r="D38" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E38" s="6" t="n">
+        <v>265</v>
+      </c>
+      <c r="F38" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G38" s="6" t="n">
+        <v>6.58</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6" t="inlineStr">
+        <is>
+          <t>2022-01-20</t>
+        </is>
+      </c>
+      <c r="B39" s="12" t="n">
+        <v>44581.40031931713</v>
+      </c>
+      <c r="C39" s="6" t="inlineStr">
+        <is>
+          <t>156_fnlrsgn</t>
+        </is>
+      </c>
+      <c r="D39" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E39" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F39" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G39" s="6" t="n">
+        <v>5.26</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="6" t="inlineStr">
+        <is>
+          <t>2022-01-28</t>
+        </is>
+      </c>
+      <c r="B40" s="12" t="n">
+        <v>44589.58420025463</v>
+      </c>
+      <c r="C40" s="6" t="inlineStr">
+        <is>
+          <t>156audit</t>
+        </is>
+      </c>
+      <c r="D40" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E40" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F40" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G40" s="6" t="n">
+        <v>5.36</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-07</t>
+        </is>
+      </c>
+      <c r="B41" s="12" t="n">
+        <v>44599.76592138889</v>
+      </c>
+      <c r="C41" s="6" t="inlineStr">
+        <is>
+          <t>secondcycle_157</t>
+        </is>
+      </c>
+      <c r="D41" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E41" s="6" t="n">
+        <v>264</v>
+      </c>
+      <c r="F41" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="G41" s="6" t="n">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-08</t>
+        </is>
+      </c>
+      <c r="B42" s="12" t="n">
+        <v>44600.41213501157</v>
+      </c>
+      <c r="C42" s="6" t="inlineStr">
+        <is>
+          <t>157_fnl</t>
+        </is>
+      </c>
+      <c r="D42" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E42" s="6" t="n">
+        <v>264</v>
+      </c>
+      <c r="F42" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="G42" s="6" t="n">
+        <v>5.94</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-24</t>
+        </is>
+      </c>
+      <c r="B43" s="12" t="n">
+        <v>44616.48866361111</v>
+      </c>
+      <c r="C43" s="6" t="inlineStr">
+        <is>
+          <t>123ghj</t>
+        </is>
+      </c>
+      <c r="D43" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E43" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="G43" s="6" t="n">
+        <v>0.28</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-24</t>
+        </is>
+      </c>
+      <c r="B44" s="12" t="n">
+        <v>44616.49095258102</v>
+      </c>
+      <c r="C44" s="6" t="inlineStr">
+        <is>
+          <t>4567ghj</t>
+        </is>
+      </c>
+      <c r="D44" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E44" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="G44" s="6" t="n">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-24</t>
+        </is>
+      </c>
+      <c r="B45" s="12" t="n">
+        <v>44616.49321247685</v>
+      </c>
+      <c r="C45" s="6" t="inlineStr">
+        <is>
+          <t>12143sdsdd</t>
+        </is>
+      </c>
+      <c r="D45" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E45" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="G45" s="6" t="n">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-24</t>
+        </is>
+      </c>
+      <c r="B46" s="12" t="n">
+        <v>44616.50936747685</v>
+      </c>
+      <c r="C46" s="6" t="inlineStr">
+        <is>
+          <t>asa2323</t>
+        </is>
+      </c>
+      <c r="D46" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E46" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="G46" s="6" t="n">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-24</t>
+        </is>
+      </c>
+      <c r="B47" s="12" t="n">
+        <v>44616.52380564815</v>
+      </c>
+      <c r="C47" s="6" t="inlineStr">
+        <is>
+          <t>www232</t>
+        </is>
+      </c>
+      <c r="D47" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E47" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="G47" s="6" t="n">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-24</t>
+        </is>
+      </c>
+      <c r="B48" s="12" t="n">
+        <v>44616.52633429398</v>
+      </c>
+      <c r="C48" s="6" t="inlineStr">
+        <is>
+          <t>3456dfg</t>
+        </is>
+      </c>
+      <c r="D48" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E48" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="G48" s="6" t="n">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-24</t>
+        </is>
+      </c>
+      <c r="B49" s="12" t="n">
+        <v>44616.53428244213</v>
+      </c>
+      <c r="C49" s="6" t="inlineStr">
+        <is>
+          <t>1345_hhh</t>
+        </is>
+      </c>
+      <c r="D49" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E49" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="G49" s="6" t="n">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-24</t>
+        </is>
+      </c>
+      <c r="B50" s="12" t="n">
+        <v>44616.54219115741</v>
+      </c>
+      <c r="C50" s="6" t="inlineStr">
+        <is>
+          <t>12324sdd</t>
+        </is>
+      </c>
+      <c r="D50" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E50" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="G50" s="6" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2022-02-24</t>
+        </is>
+      </c>
+      <c r="B51" s="12" t="n">
+        <v>44616.55075899666</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>asa2332</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>269</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>269</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.26</v>
+      </c>
+    </row>
     <row r="1048574" ht="12.8" customHeight="1" s="7"/>
     <row r="1048575" ht="12.8" customHeight="1" s="7"/>
     <row r="1048576" ht="12.8" customHeight="1" s="7"/>
@@ -1352,7 +1914,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
@@ -1812,6 +2374,141 @@
         <v>5.28</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>2021-11-18</t>
+        </is>
+      </c>
+      <c r="B17" s="12" t="n">
+        <v>44518.57093840278</v>
+      </c>
+      <c r="C17" s="6" t="inlineStr">
+        <is>
+          <t>153_beta</t>
+        </is>
+      </c>
+      <c r="D17" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F17" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6" t="n">
+        <v>6.57</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="inlineStr">
+        <is>
+          <t>2021-12-06</t>
+        </is>
+      </c>
+      <c r="B18" s="12" t="n">
+        <v>44536.54220427083</v>
+      </c>
+      <c r="C18" s="6" t="inlineStr">
+        <is>
+          <t>154_beta</t>
+        </is>
+      </c>
+      <c r="D18" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <v>266</v>
+      </c>
+      <c r="F18" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G18" s="6" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>2021-12-23</t>
+        </is>
+      </c>
+      <c r="B19" s="12" t="n">
+        <v>44553.51663828704</v>
+      </c>
+      <c r="C19" s="6" t="inlineStr">
+        <is>
+          <t>155_beta</t>
+        </is>
+      </c>
+      <c r="D19" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E19" s="6" t="n">
+        <v>264</v>
+      </c>
+      <c r="F19" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="G19" s="6" t="n">
+        <v>5.56</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>2022-01-20</t>
+        </is>
+      </c>
+      <c r="B20" s="12" t="n">
+        <v>44581.53406202546</v>
+      </c>
+      <c r="C20" s="6" t="inlineStr">
+        <is>
+          <t>156_beta</t>
+        </is>
+      </c>
+      <c r="D20" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E20" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F20" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6" t="n">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-08</t>
+        </is>
+      </c>
+      <c r="B21" s="12" t="n">
+        <v>44600.62059473379</v>
+      </c>
+      <c r="C21" s="6" t="inlineStr">
+        <is>
+          <t>157_beta</t>
+        </is>
+      </c>
+      <c r="D21" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E21" s="6" t="n">
+        <v>262</v>
+      </c>
+      <c r="F21" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="G21" s="6" t="n">
+        <v>14.03</v>
+      </c>
+    </row>
     <row r="1048576" ht="15" customHeight="1" s="7"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -1826,7 +2523,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
@@ -2638,30 +3335,246 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="6" t="inlineStr">
         <is>
           <t>2021-10-28</t>
         </is>
       </c>
       <c r="B30" s="12" t="n">
-        <v>44497.85545837627</v>
-      </c>
-      <c r="C30" t="inlineStr">
+        <v>44497.85545837963</v>
+      </c>
+      <c r="C30" s="6" t="inlineStr">
         <is>
           <t>152_livetest</t>
         </is>
       </c>
-      <c r="D30" t="n">
-        <v>269</v>
-      </c>
-      <c r="E30" t="n">
+      <c r="D30" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E30" s="6" t="n">
         <v>268</v>
       </c>
-      <c r="F30" t="n">
+      <c r="F30" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G30" t="n">
+      <c r="G30" s="6" t="n">
         <v>4.63</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="inlineStr">
+        <is>
+          <t>2021-11-23</t>
+        </is>
+      </c>
+      <c r="B31" s="12" t="n">
+        <v>44523.4393272338</v>
+      </c>
+      <c r="C31" s="6" t="inlineStr">
+        <is>
+          <t>153_live</t>
+        </is>
+      </c>
+      <c r="D31" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E31" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F31" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="6" t="n">
+        <v>4.97</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="inlineStr">
+        <is>
+          <t>2021-12-06</t>
+        </is>
+      </c>
+      <c r="B32" s="12" t="n">
+        <v>44536.86230123843</v>
+      </c>
+      <c r="C32" s="6" t="inlineStr">
+        <is>
+          <t>154_live</t>
+        </is>
+      </c>
+      <c r="D32" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E32" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F32" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" s="6" t="n">
+        <v>5.44</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>2021-12-09</t>
+        </is>
+      </c>
+      <c r="B33" s="12" t="n">
+        <v>44539.78338771991</v>
+      </c>
+      <c r="C33" s="6" t="inlineStr">
+        <is>
+          <t>154htfxx</t>
+        </is>
+      </c>
+      <c r="D33" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E33" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F33" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="6" t="n">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t>2021-12-23</t>
+        </is>
+      </c>
+      <c r="B34" s="12" t="n">
+        <v>44553.78829818287</v>
+      </c>
+      <c r="C34" s="6" t="inlineStr">
+        <is>
+          <t>155_live</t>
+        </is>
+      </c>
+      <c r="D34" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E34" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F34" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" s="6" t="n">
+        <v>4.57</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="inlineStr">
+        <is>
+          <t>2021-12-27</t>
+        </is>
+      </c>
+      <c r="B35" s="12" t="n">
+        <v>44557.70460170139</v>
+      </c>
+      <c r="C35" s="6" t="inlineStr">
+        <is>
+          <t>155hftfxx</t>
+        </is>
+      </c>
+      <c r="D35" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E35" s="6" t="n">
+        <v>264</v>
+      </c>
+      <c r="F35" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="G35" s="6" t="n">
+        <v>5.06</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="inlineStr">
+        <is>
+          <t>2022-01-20</t>
+        </is>
+      </c>
+      <c r="B36" s="12" t="n">
+        <v>44581.81741920139</v>
+      </c>
+      <c r="C36" s="6" t="inlineStr">
+        <is>
+          <t>156_live</t>
+        </is>
+      </c>
+      <c r="D36" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E36" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F36" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="6" t="n">
+        <v>4.14</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-08</t>
+        </is>
+      </c>
+      <c r="B37" s="12" t="n">
+        <v>44600.85738260417</v>
+      </c>
+      <c r="C37" s="6" t="inlineStr">
+        <is>
+          <t>157_live</t>
+        </is>
+      </c>
+      <c r="D37" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E37" s="6" t="n">
+        <v>265</v>
+      </c>
+      <c r="F37" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G37" s="6" t="n">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-24</t>
+        </is>
+      </c>
+      <c r="B38" s="12" t="n">
+        <v>44616.52923978009</v>
+      </c>
+      <c r="C38" s="6" t="inlineStr">
+        <is>
+          <t>453_gj</t>
+        </is>
+      </c>
+      <c r="D38" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E38" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="G38" s="6" t="n">
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes in upload count/close
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
@@ -1872,30 +1872,111 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="A51" s="6" t="inlineStr">
         <is>
           <t>2022-02-24</t>
         </is>
       </c>
       <c r="B51" s="12" t="n">
-        <v>44616.55075899666</v>
-      </c>
-      <c r="C51" t="inlineStr">
+        <v>44616.55075899306</v>
+      </c>
+      <c r="C51" s="6" t="inlineStr">
         <is>
           <t>asa2332</t>
         </is>
       </c>
-      <c r="D51" t="n">
-        <v>269</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" t="n">
-        <v>269</v>
-      </c>
-      <c r="G51" t="n">
+      <c r="D51" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E51" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="G51" s="6" t="n">
         <v>0.26</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-24</t>
+        </is>
+      </c>
+      <c r="B52" s="12" t="n">
+        <v>44616.70045383102</v>
+      </c>
+      <c r="C52" s="6" t="inlineStr">
+        <is>
+          <t>test1234</t>
+        </is>
+      </c>
+      <c r="D52" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E52" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F52" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="G52" s="6" t="n">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="inlineStr">
+        <is>
+          <t>2022-02-25</t>
+        </is>
+      </c>
+      <c r="B53" s="12" t="n">
+        <v>44617.49754053241</v>
+      </c>
+      <c r="C53" s="6" t="inlineStr">
+        <is>
+          <t>test158</t>
+        </is>
+      </c>
+      <c r="D53" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E53" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F53" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G53" s="6" t="n">
+        <v>5.45</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2022-02-25</t>
+        </is>
+      </c>
+      <c r="B54" s="12" t="n">
+        <v>44617.52886187014</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>test158</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>269</v>
+      </c>
+      <c r="E54" t="n">
+        <v>74</v>
+      </c>
+      <c r="F54" t="n">
+        <v>195</v>
+      </c>
+      <c r="G54" t="n">
+        <v>3.21</v>
       </c>
     </row>
     <row r="1048574" ht="12.8" customHeight="1" s="7"/>

</xml_diff>

<commit_message>
Microsite Education Script completed
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="AMSIN" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="BETA" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="AMS" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="INDIA" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMSIN" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BETA" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMS" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="INDIA" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
@@ -2384,6 +2384,276 @@
         <v>4.78</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" s="6" t="inlineStr">
+        <is>
+          <t>2022-07-19</t>
+        </is>
+      </c>
+      <c r="B70" s="12" t="n">
+        <v>44761.50344545139</v>
+      </c>
+      <c r="C70" s="6" t="inlineStr">
+        <is>
+          <t>3133d</t>
+        </is>
+      </c>
+      <c r="D70" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E70" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="G70" s="6" t="n">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="6" t="inlineStr">
+        <is>
+          <t>2022-07-19</t>
+        </is>
+      </c>
+      <c r="B71" s="12" t="n">
+        <v>44761.50466866898</v>
+      </c>
+      <c r="C71" s="6" t="inlineStr">
+        <is>
+          <t>124s</t>
+        </is>
+      </c>
+      <c r="D71" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E71" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="G71" s="6" t="n">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="6" t="inlineStr">
+        <is>
+          <t>2022-07-19</t>
+        </is>
+      </c>
+      <c r="B72" s="12" t="n">
+        <v>44761.50676752315</v>
+      </c>
+      <c r="C72" s="6" t="inlineStr">
+        <is>
+          <t>131ds</t>
+        </is>
+      </c>
+      <c r="D72" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E72" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="G72" s="6" t="n">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="6" t="inlineStr">
+        <is>
+          <t>2022-08-02</t>
+        </is>
+      </c>
+      <c r="B73" s="12" t="n">
+        <v>44775.63534686343</v>
+      </c>
+      <c r="C73" s="6" t="inlineStr">
+        <is>
+          <t>165_fstcycle</t>
+        </is>
+      </c>
+      <c r="D73" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E73" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F73" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G73" s="6" t="n">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="6" t="inlineStr">
+        <is>
+          <t>2022-08-04</t>
+        </is>
+      </c>
+      <c r="B74" s="12" t="n">
+        <v>44777.37942087963</v>
+      </c>
+      <c r="C74" s="6" t="inlineStr">
+        <is>
+          <t>165_finalrun</t>
+        </is>
+      </c>
+      <c r="D74" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E74" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F74" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G74" s="6" t="n">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="6" t="inlineStr">
+        <is>
+          <t>2022-08-22</t>
+        </is>
+      </c>
+      <c r="B75" s="12" t="n">
+        <v>44795.64787594907</v>
+      </c>
+      <c r="C75" s="6" t="inlineStr">
+        <is>
+          <t>166fstcycle</t>
+        </is>
+      </c>
+      <c r="D75" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E75" s="6" t="n">
+        <v>264</v>
+      </c>
+      <c r="F75" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="G75" s="6" t="n">
+        <v>4.79</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="6" t="inlineStr">
+        <is>
+          <t>2022-08-23</t>
+        </is>
+      </c>
+      <c r="B76" s="12" t="n">
+        <v>44796.65294547454</v>
+      </c>
+      <c r="C76" s="6" t="inlineStr">
+        <is>
+          <t>166scndcyle</t>
+        </is>
+      </c>
+      <c r="D76" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E76" s="6" t="n">
+        <v>211</v>
+      </c>
+      <c r="F76" s="6" t="n">
+        <v>58</v>
+      </c>
+      <c r="G76" s="6" t="n">
+        <v>16.81</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="6" t="inlineStr">
+        <is>
+          <t>2022-08-23</t>
+        </is>
+      </c>
+      <c r="B77" s="12" t="n">
+        <v>44796.8913643287</v>
+      </c>
+      <c r="C77" s="6" t="inlineStr">
+        <is>
+          <t>166cyclescnd</t>
+        </is>
+      </c>
+      <c r="D77" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E77" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F77" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G77" s="6" t="n">
+        <v>5.19</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="6" t="inlineStr">
+        <is>
+          <t>2022-08-25</t>
+        </is>
+      </c>
+      <c r="B78" s="12" t="n">
+        <v>44798.86474379629</v>
+      </c>
+      <c r="C78" s="6" t="inlineStr">
+        <is>
+          <t>hotfix166</t>
+        </is>
+      </c>
+      <c r="D78" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E78" s="6" t="n">
+        <v>266</v>
+      </c>
+      <c r="F78" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G78" s="6" t="n">
+        <v>4.86</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="6" t="inlineStr">
+        <is>
+          <t>2022-08-28</t>
+        </is>
+      </c>
+      <c r="B79" s="12" t="n">
+        <v>44801.74069929398</v>
+      </c>
+      <c r="C79" s="6" t="inlineStr">
+        <is>
+          <t>sundhtfx166</t>
+        </is>
+      </c>
+      <c r="D79" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E79" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F79" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G79" s="6" t="n">
+        <v>4.83</v>
+      </c>
+    </row>
     <row r="1048574" ht="12.8" customHeight="1" s="7"/>
     <row r="1048575" ht="12.8" customHeight="1" s="7"/>
     <row r="1048576" ht="12.8" customHeight="1" s="7"/>
@@ -2400,7 +2670,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
@@ -3130,6 +3400,60 @@
         <v>4.2</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" s="6" t="inlineStr">
+        <is>
+          <t>2022-08-04</t>
+        </is>
+      </c>
+      <c r="B27" s="12" t="n">
+        <v>44777.54708997686</v>
+      </c>
+      <c r="C27" s="6" t="inlineStr">
+        <is>
+          <t>165beta</t>
+        </is>
+      </c>
+      <c r="D27" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E27" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F27" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" s="6" t="n">
+        <v>4.88</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>2022-08-24</t>
+        </is>
+      </c>
+      <c r="B28" s="12" t="n">
+        <v>44797.51160618055</v>
+      </c>
+      <c r="C28" s="6" t="inlineStr">
+        <is>
+          <t>166_beta</t>
+        </is>
+      </c>
+      <c r="D28" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E28" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F28" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="6" t="n">
+        <v>4.32</v>
+      </c>
+    </row>
     <row r="1048576" ht="15" customHeight="1" s="7"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -3144,7 +3468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
@@ -4361,29 +4685,137 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
+      <c r="A45" s="6" t="inlineStr">
         <is>
           <t>2022-07-14</t>
         </is>
       </c>
       <c r="B45" s="12" t="n">
-        <v>44756.80692301049</v>
-      </c>
-      <c r="C45" t="inlineStr">
+        <v>44756.80692300926</v>
+      </c>
+      <c r="C45" s="6" t="inlineStr">
         <is>
           <t>164_live</t>
         </is>
       </c>
-      <c r="D45" t="n">
-        <v>269</v>
-      </c>
-      <c r="E45" t="n">
+      <c r="D45" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E45" s="6" t="n">
         <v>268</v>
       </c>
-      <c r="F45" t="n">
+      <c r="F45" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G45" t="n">
+      <c r="G45" s="6" t="n">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="6" t="inlineStr">
+        <is>
+          <t>2022-08-04</t>
+        </is>
+      </c>
+      <c r="B46" s="12" t="n">
+        <v>44777.80374391204</v>
+      </c>
+      <c r="C46" s="6" t="inlineStr">
+        <is>
+          <t>165_live</t>
+        </is>
+      </c>
+      <c r="D46" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E46" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F46" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" s="6" t="n">
+        <v>3.68</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="6" t="inlineStr">
+        <is>
+          <t>2022-08-24</t>
+        </is>
+      </c>
+      <c r="B47" s="12" t="n">
+        <v>44797.90853664352</v>
+      </c>
+      <c r="C47" s="6" t="inlineStr">
+        <is>
+          <t>166_live</t>
+        </is>
+      </c>
+      <c r="D47" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E47" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F47" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" s="6" t="n">
+        <v>3.68</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="6" t="inlineStr">
+        <is>
+          <t>2022-08-25</t>
+        </is>
+      </c>
+      <c r="B48" s="12" t="n">
+        <v>44798.87621078704</v>
+      </c>
+      <c r="C48" s="6" t="inlineStr">
+        <is>
+          <t>166hotfix</t>
+        </is>
+      </c>
+      <c r="D48" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E48" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F48" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" s="6" t="n">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2022-08-28</t>
+        </is>
+      </c>
+      <c r="B49" s="12" t="n">
+        <v>44801.86460017557</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>166sundyhtfx</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>269</v>
+      </c>
+      <c r="E49" t="n">
+        <v>268</v>
+      </c>
+      <c r="F49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G49" t="n">
         <v>3.8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
OCR FLOW COMPLETED/MODIFICATION IN EDUCATION FLOW
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -3468,7 +3468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
@@ -4793,30 +4793,57 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
+      <c r="A49" s="6" t="inlineStr">
         <is>
           <t>2022-08-28</t>
         </is>
       </c>
       <c r="B49" s="12" t="n">
-        <v>44801.86460017557</v>
-      </c>
-      <c r="C49" t="inlineStr">
+        <v>44801.86460017361</v>
+      </c>
+      <c r="C49" s="6" t="inlineStr">
         <is>
           <t>166sundyhtfx</t>
         </is>
       </c>
-      <c r="D49" t="n">
-        <v>269</v>
-      </c>
-      <c r="E49" t="n">
+      <c r="D49" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E49" s="6" t="n">
         <v>268</v>
       </c>
-      <c r="F49" t="n">
+      <c r="F49" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G49" t="n">
+      <c r="G49" s="6" t="n">
         <v>3.8</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2022-09-01</t>
+        </is>
+      </c>
+      <c r="B50" s="12" t="n">
+        <v>44805.75095284091</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>htf166sep</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>269</v>
+      </c>
+      <c r="E50" t="n">
+        <v>264</v>
+      </c>
+      <c r="F50" t="n">
+        <v>5</v>
+      </c>
+      <c r="G50" t="n">
+        <v>4.87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Razorpay Script Completed / Some Bug fixes in registartion page flows
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -3468,7 +3468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
@@ -4820,30 +4820,57 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
+      <c r="A50" s="6" t="inlineStr">
         <is>
           <t>2022-09-01</t>
         </is>
       </c>
       <c r="B50" s="12" t="n">
-        <v>44805.75095284091</v>
-      </c>
-      <c r="C50" t="inlineStr">
+        <v>44805.75095283565</v>
+      </c>
+      <c r="C50" s="6" t="inlineStr">
         <is>
           <t>htf166sep</t>
         </is>
       </c>
-      <c r="D50" t="n">
-        <v>269</v>
-      </c>
-      <c r="E50" t="n">
+      <c r="D50" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E50" s="6" t="n">
         <v>264</v>
       </c>
-      <c r="F50" t="n">
+      <c r="F50" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="G50" t="n">
+      <c r="G50" s="6" t="n">
         <v>4.87</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2022-09-06</t>
+        </is>
+      </c>
+      <c r="B51" s="12" t="n">
+        <v>44810.92359607792</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>htfx166tue</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>269</v>
+      </c>
+      <c r="E51" t="n">
+        <v>268</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G51" t="n">
+        <v>3.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Microsite scripts support to Beta server
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
@@ -2654,6 +2654,87 @@
         <v>4.83</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" s="6" t="inlineStr">
+        <is>
+          <t>2022-09-16</t>
+        </is>
+      </c>
+      <c r="B80" s="12" t="n">
+        <v>44820.6029044676</v>
+      </c>
+      <c r="C80" s="6" t="inlineStr">
+        <is>
+          <t>fstcyc167</t>
+        </is>
+      </c>
+      <c r="D80" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E80" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F80" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G80" s="6" t="n">
+        <v>5.46</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="6" t="inlineStr">
+        <is>
+          <t>2022-09-19</t>
+        </is>
+      </c>
+      <c r="B81" s="12" t="n">
+        <v>44823.61774643519</v>
+      </c>
+      <c r="C81" s="6" t="inlineStr">
+        <is>
+          <t>scndcycle167</t>
+        </is>
+      </c>
+      <c r="D81" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E81" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F81" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G81" s="6" t="n">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="6" t="inlineStr">
+        <is>
+          <t>2022-09-20</t>
+        </is>
+      </c>
+      <c r="B82" s="12" t="n">
+        <v>44824.36184575231</v>
+      </c>
+      <c r="C82" s="6" t="inlineStr">
+        <is>
+          <t>finalrun167</t>
+        </is>
+      </c>
+      <c r="D82" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E82" s="6" t="n">
+        <v>262</v>
+      </c>
+      <c r="F82" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="G82" s="6" t="n">
+        <v>7.66</v>
+      </c>
+    </row>
     <row r="1048574" ht="12.8" customHeight="1" s="7"/>
     <row r="1048575" ht="12.8" customHeight="1" s="7"/>
     <row r="1048576" ht="12.8" customHeight="1" s="7"/>
@@ -2670,7 +2751,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
@@ -3454,6 +3535,33 @@
         <v>4.32</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2022-09-20</t>
+        </is>
+      </c>
+      <c r="B29" s="12" t="n">
+        <v>44824.50985645134</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>beta167</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>269</v>
+      </c>
+      <c r="E29" t="n">
+        <v>268</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" t="n">
+        <v>4.22</v>
+      </c>
+    </row>
     <row r="1048576" ht="15" customHeight="1" s="7"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -3468,7 +3576,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
@@ -4847,30 +4955,57 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
+      <c r="A51" s="6" t="inlineStr">
         <is>
           <t>2022-09-06</t>
         </is>
       </c>
       <c r="B51" s="12" t="n">
-        <v>44810.92359607792</v>
-      </c>
-      <c r="C51" t="inlineStr">
+        <v>44810.92359607639</v>
+      </c>
+      <c r="C51" s="6" t="inlineStr">
         <is>
           <t>htfx166tue</t>
         </is>
       </c>
-      <c r="D51" t="n">
-        <v>269</v>
-      </c>
-      <c r="E51" t="n">
+      <c r="D51" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E51" s="6" t="n">
         <v>268</v>
       </c>
-      <c r="F51" t="n">
+      <c r="F51" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G51" t="n">
+      <c r="G51" s="6" t="n">
         <v>3.67</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="6" t="inlineStr">
+        <is>
+          <t>2022-09-14</t>
+        </is>
+      </c>
+      <c r="B52" s="12" t="n">
+        <v>44818.40202697917</v>
+      </c>
+      <c r="C52" s="6" t="inlineStr">
+        <is>
+          <t>livehtfxsep166</t>
+        </is>
+      </c>
+      <c r="D52" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E52" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F52" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G52" s="6" t="n">
+        <v>3.92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aadhar flow completed and added
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -3981,7 +3981,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
@@ -5792,30 +5792,84 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr">
+      <c r="A67" s="6" t="inlineStr">
         <is>
           <t>2023-01-25</t>
         </is>
       </c>
       <c r="B67" s="12" t="n">
-        <v>44951.72762466512</v>
-      </c>
-      <c r="C67" t="inlineStr">
+        <v>44951.72762466435</v>
+      </c>
+      <c r="C67" s="6" t="inlineStr">
         <is>
           <t>htfx172wed</t>
         </is>
       </c>
-      <c r="D67" t="n">
-        <v>269</v>
-      </c>
-      <c r="E67" t="n">
-        <v>269</v>
-      </c>
-      <c r="F67" t="n">
-        <v>0</v>
-      </c>
-      <c r="G67" t="n">
+      <c r="D67" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E67" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F67" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" s="6" t="n">
         <v>3.93</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="6" t="inlineStr">
+        <is>
+          <t>2023-02-03</t>
+        </is>
+      </c>
+      <c r="B68" s="12" t="n">
+        <v>44960.6133114699</v>
+      </c>
+      <c r="C68" s="6" t="inlineStr">
+        <is>
+          <t>172htfxthree</t>
+        </is>
+      </c>
+      <c r="D68" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E68" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F68" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" s="6" t="n">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2023-02-06</t>
+        </is>
+      </c>
+      <c r="B69" s="12" t="n">
+        <v>44963.75031220534</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>172fourhtfx</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>269</v>
+      </c>
+      <c r="E69" t="n">
+        <v>269</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>4.31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issues fixes and reports
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G93"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
@@ -3032,6 +3032,60 @@
         <v>5.17</v>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" s="6" t="inlineStr">
+        <is>
+          <t>2023-02-16</t>
+        </is>
+      </c>
+      <c r="B94" s="12" t="n">
+        <v>44973.76391283565</v>
+      </c>
+      <c r="C94" s="6" t="inlineStr">
+        <is>
+          <t>173cyclefst</t>
+        </is>
+      </c>
+      <c r="D94" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E94" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F94" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G94" s="6" t="n">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="6" t="inlineStr">
+        <is>
+          <t>2023-02-20</t>
+        </is>
+      </c>
+      <c r="B95" s="12" t="n">
+        <v>44977.39481481481</v>
+      </c>
+      <c r="C95" s="6" t="inlineStr">
+        <is>
+          <t>173fnlrun</t>
+        </is>
+      </c>
+      <c r="D95" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E95" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F95" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G95" s="6" t="n">
+        <v>4.6</v>
+      </c>
+    </row>
     <row r="1048574" ht="12.8" customHeight="1" s="7"/>
     <row r="1048575" ht="12.8" customHeight="1" s="7"/>
     <row r="1048576" ht="12.8" customHeight="1" s="7"/>
@@ -3048,7 +3102,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
@@ -3967,6 +4021,33 @@
         <v>4.36</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t>2023-02-20</t>
+        </is>
+      </c>
+      <c r="B34" s="12" t="n">
+        <v>44977.57882420139</v>
+      </c>
+      <c r="C34" s="6" t="inlineStr">
+        <is>
+          <t>173beta</t>
+        </is>
+      </c>
+      <c r="D34" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E34" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F34" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G34" s="6" t="n">
+        <v>4.06</v>
+      </c>
+    </row>
     <row r="1048576" ht="15" customHeight="1" s="7"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -3981,7 +4062,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
@@ -5846,30 +5927,57 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
+      <c r="A69" s="6" t="inlineStr">
         <is>
           <t>2023-02-06</t>
         </is>
       </c>
       <c r="B69" s="12" t="n">
-        <v>44963.75031220534</v>
-      </c>
-      <c r="C69" t="inlineStr">
+        <v>44963.75031221065</v>
+      </c>
+      <c r="C69" s="6" t="inlineStr">
         <is>
           <t>172fourhtfx</t>
         </is>
       </c>
-      <c r="D69" t="n">
-        <v>269</v>
-      </c>
-      <c r="E69" t="n">
-        <v>269</v>
-      </c>
-      <c r="F69" t="n">
-        <v>0</v>
-      </c>
-      <c r="G69" t="n">
+      <c r="D69" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E69" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F69" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" s="6" t="n">
         <v>4.31</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2023-02-20</t>
+        </is>
+      </c>
+      <c r="B70" s="12" t="n">
+        <v>44977.83047720879</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>live173</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>269</v>
+      </c>
+      <c r="E70" t="n">
+        <v>268</v>
+      </c>
+      <c r="F70" t="n">
+        <v>1</v>
+      </c>
+      <c r="G70" t="n">
+        <v>4.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work Profile and new tenant support
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G95"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
@@ -3086,6 +3086,222 @@
         <v>4.6</v>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" s="6" t="inlineStr">
+        <is>
+          <t>2023-02-23</t>
+        </is>
+      </c>
+      <c r="B96" s="12" t="n">
+        <v>44980.75622256944</v>
+      </c>
+      <c r="C96" s="6" t="inlineStr">
+        <is>
+          <t>173hhttffxx</t>
+        </is>
+      </c>
+      <c r="D96" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E96" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F96" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G96" s="6" t="n">
+        <v>5.32</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="6" t="inlineStr">
+        <is>
+          <t>2023-03-09</t>
+        </is>
+      </c>
+      <c r="B97" s="12" t="n">
+        <v>44994.57150388889</v>
+      </c>
+      <c r="C97" s="6" t="inlineStr">
+        <is>
+          <t>174fstcycle</t>
+        </is>
+      </c>
+      <c r="D97" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E97" s="6" t="n">
+        <v>264</v>
+      </c>
+      <c r="F97" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="G97" s="6" t="n">
+        <v>6.28</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="6" t="inlineStr">
+        <is>
+          <t>2023-03-10</t>
+        </is>
+      </c>
+      <c r="B98" s="12" t="n">
+        <v>44995.78329828704</v>
+      </c>
+      <c r="C98" s="6" t="inlineStr">
+        <is>
+          <t>174ffiinnalrun</t>
+        </is>
+      </c>
+      <c r="D98" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E98" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F98" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G98" s="6" t="n">
+        <v>5.98</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="6" t="inlineStr">
+        <is>
+          <t>2023-03-13</t>
+        </is>
+      </c>
+      <c r="B99" s="12" t="n">
+        <v>44998.46071991898</v>
+      </c>
+      <c r="C99" s="6" t="inlineStr">
+        <is>
+          <t>174finalrun</t>
+        </is>
+      </c>
+      <c r="D99" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E99" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F99" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G99" s="6" t="n">
+        <v>4.79</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="6" t="inlineStr">
+        <is>
+          <t>2023-03-28</t>
+        </is>
+      </c>
+      <c r="B100" s="12" t="n">
+        <v>45013.52588585648</v>
+      </c>
+      <c r="C100" s="6" t="inlineStr">
+        <is>
+          <t>175prerun</t>
+        </is>
+      </c>
+      <c r="D100" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E100" s="6" t="n">
+        <v>266</v>
+      </c>
+      <c r="F100" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G100" s="6" t="n">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="6" t="inlineStr">
+        <is>
+          <t>2023-03-30</t>
+        </is>
+      </c>
+      <c r="B101" s="12" t="n">
+        <v>45015.70615905093</v>
+      </c>
+      <c r="C101" s="6" t="inlineStr">
+        <is>
+          <t>175scndcyc</t>
+        </is>
+      </c>
+      <c r="D101" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E101" s="6" t="n">
+        <v>263</v>
+      </c>
+      <c r="F101" s="6" t="n">
+        <v>6</v>
+      </c>
+      <c r="G101" s="6" t="n">
+        <v>6.69</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="6" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="B102" s="12" t="n">
+        <v>45016.44203090278</v>
+      </c>
+      <c r="C102" s="6" t="inlineStr">
+        <is>
+          <t>175fnlrun</t>
+        </is>
+      </c>
+      <c r="D102" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E102" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F102" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G102" s="6" t="n">
+        <v>5.23</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2023-04-12</t>
+        </is>
+      </c>
+      <c r="B103" s="12" t="n">
+        <v>45028.45964890953</v>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>176fstrtail</t>
+        </is>
+      </c>
+      <c r="D103" t="n">
+        <v>269</v>
+      </c>
+      <c r="E103" t="n">
+        <v>260</v>
+      </c>
+      <c r="F103" t="n">
+        <v>9</v>
+      </c>
+      <c r="G103" t="n">
+        <v>6.04</v>
+      </c>
+    </row>
     <row r="1048574" ht="12.8" customHeight="1" s="7"/>
     <row r="1048575" ht="12.8" customHeight="1" s="7"/>
     <row r="1048576" ht="12.8" customHeight="1" s="7"/>
@@ -3102,7 +3318,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
@@ -4048,6 +4264,60 @@
         <v>4.06</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" s="6" t="inlineStr">
+        <is>
+          <t>2023-03-13</t>
+        </is>
+      </c>
+      <c r="B35" s="12" t="n">
+        <v>44998.52453083333</v>
+      </c>
+      <c r="C35" s="6" t="inlineStr">
+        <is>
+          <t>174beta</t>
+        </is>
+      </c>
+      <c r="D35" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E35" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F35" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G35" s="6" t="n">
+        <v>3.92</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="B36" s="12" t="n">
+        <v>45016.52234857639</v>
+      </c>
+      <c r="C36" s="6" t="inlineStr">
+        <is>
+          <t>175beta</t>
+        </is>
+      </c>
+      <c r="D36" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E36" s="6" t="n">
+        <v>265</v>
+      </c>
+      <c r="F36" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G36" s="6" t="n">
+        <v>4.52</v>
+      </c>
+    </row>
     <row r="1048576" ht="15" customHeight="1" s="7"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -4062,7 +4332,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
@@ -5954,30 +6224,192 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
+      <c r="A70" s="6" t="inlineStr">
         <is>
           <t>2023-02-20</t>
         </is>
       </c>
       <c r="B70" s="12" t="n">
-        <v>44977.83047720879</v>
-      </c>
-      <c r="C70" t="inlineStr">
+        <v>44977.83047721065</v>
+      </c>
+      <c r="C70" s="6" t="inlineStr">
         <is>
           <t>live173</t>
         </is>
       </c>
-      <c r="D70" t="n">
-        <v>269</v>
-      </c>
-      <c r="E70" t="n">
+      <c r="D70" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E70" s="6" t="n">
         <v>268</v>
       </c>
-      <c r="F70" t="n">
+      <c r="F70" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="G70" t="n">
+      <c r="G70" s="6" t="n">
         <v>4.05</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="6" t="inlineStr">
+        <is>
+          <t>2023-02-23</t>
+        </is>
+      </c>
+      <c r="B71" s="12" t="n">
+        <v>44980.83663085648</v>
+      </c>
+      <c r="C71" s="6" t="inlineStr">
+        <is>
+          <t>173htfxbulkschedule</t>
+        </is>
+      </c>
+      <c r="D71" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E71" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F71" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" s="6" t="n">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="6" t="inlineStr">
+        <is>
+          <t>2023-03-01</t>
+        </is>
+      </c>
+      <c r="B72" s="12" t="n">
+        <v>44986.68783164352</v>
+      </c>
+      <c r="C72" s="6" t="inlineStr">
+        <is>
+          <t>173angularvrs</t>
+        </is>
+      </c>
+      <c r="D72" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E72" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F72" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" s="6" t="n">
+        <v>3.78</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="6" t="inlineStr">
+        <is>
+          <t>2023-03-02</t>
+        </is>
+      </c>
+      <c r="B73" s="12" t="n">
+        <v>44987.43015282408</v>
+      </c>
+      <c r="C73" s="6" t="inlineStr">
+        <is>
+          <t>liveangular173</t>
+        </is>
+      </c>
+      <c r="D73" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E73" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F73" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" s="6" t="n">
+        <v>4.16</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="6" t="inlineStr">
+        <is>
+          <t>2023-03-07</t>
+        </is>
+      </c>
+      <c r="B74" s="12" t="n">
+        <v>44992.73899635416</v>
+      </c>
+      <c r="C74" s="6" t="inlineStr">
+        <is>
+          <t>174htfxmar</t>
+        </is>
+      </c>
+      <c r="D74" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E74" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F74" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G74" s="6" t="n">
+        <v>4.03</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="6" t="inlineStr">
+        <is>
+          <t>2023-03-13</t>
+        </is>
+      </c>
+      <c r="B75" s="12" t="n">
+        <v>44998.83213166667</v>
+      </c>
+      <c r="C75" s="6" t="inlineStr">
+        <is>
+          <t>174live</t>
+        </is>
+      </c>
+      <c r="D75" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E75" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F75" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G75" s="6" t="n">
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="6" t="inlineStr">
+        <is>
+          <t>2023-03-31</t>
+        </is>
+      </c>
+      <c r="B76" s="12" t="n">
+        <v>45016.78996877315</v>
+      </c>
+      <c r="C76" s="6" t="inlineStr">
+        <is>
+          <t>175live</t>
+        </is>
+      </c>
+      <c r="D76" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E76" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F76" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G76" s="6" t="n">
+        <v>4.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Custom properties -bug fixes
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G103"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
@@ -3276,30 +3276,84 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr">
+      <c r="A103" s="6" t="inlineStr">
         <is>
           <t>2023-04-12</t>
         </is>
       </c>
       <c r="B103" s="12" t="n">
-        <v>45028.45964890953</v>
-      </c>
-      <c r="C103" t="inlineStr">
+        <v>45028.45964891204</v>
+      </c>
+      <c r="C103" s="6" t="inlineStr">
         <is>
           <t>176fstrtail</t>
         </is>
       </c>
-      <c r="D103" t="n">
-        <v>269</v>
-      </c>
-      <c r="E103" t="n">
+      <c r="D103" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E103" s="6" t="n">
         <v>260</v>
       </c>
-      <c r="F103" t="n">
+      <c r="F103" s="6" t="n">
         <v>9</v>
       </c>
-      <c r="G103" t="n">
+      <c r="G103" s="6" t="n">
         <v>6.04</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="6" t="inlineStr">
+        <is>
+          <t>2023-04-18</t>
+        </is>
+      </c>
+      <c r="B104" s="12" t="n">
+        <v>45034.52080172454</v>
+      </c>
+      <c r="C104" s="6" t="inlineStr">
+        <is>
+          <t>176firsttrail</t>
+        </is>
+      </c>
+      <c r="D104" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E104" s="6" t="n">
+        <v>264</v>
+      </c>
+      <c r="F104" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="G104" s="6" t="n">
+        <v>5.64</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2023-04-18</t>
+        </is>
+      </c>
+      <c r="B105" s="12" t="n">
+        <v>45034.62628673139</v>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>176fstscndtr</t>
+        </is>
+      </c>
+      <c r="D105" t="n">
+        <v>269</v>
+      </c>
+      <c r="E105" t="n">
+        <v>261</v>
+      </c>
+      <c r="F105" t="n">
+        <v>8</v>
+      </c>
+      <c r="G105" t="n">
+        <v>5.11</v>
       </c>
     </row>
     <row r="1048574" ht="12.8" customHeight="1" s="7"/>

</xml_diff>

<commit_message>
New tenant support in live
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G105"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
@@ -3330,30 +3330,84 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="inlineStr">
+      <c r="A105" s="6" t="inlineStr">
         <is>
           <t>2023-04-18</t>
         </is>
       </c>
       <c r="B105" s="12" t="n">
-        <v>45034.62628673139</v>
-      </c>
-      <c r="C105" t="inlineStr">
+        <v>45034.62628673611</v>
+      </c>
+      <c r="C105" s="6" t="inlineStr">
         <is>
           <t>176fstscndtr</t>
         </is>
       </c>
-      <c r="D105" t="n">
-        <v>269</v>
-      </c>
-      <c r="E105" t="n">
+      <c r="D105" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E105" s="6" t="n">
         <v>261</v>
       </c>
-      <c r="F105" t="n">
+      <c r="F105" s="6" t="n">
         <v>8</v>
       </c>
-      <c r="G105" t="n">
+      <c r="G105" s="6" t="n">
         <v>5.11</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="6" t="inlineStr">
+        <is>
+          <t>2023-04-19</t>
+        </is>
+      </c>
+      <c r="B106" s="12" t="n">
+        <v>45035.6895700926</v>
+      </c>
+      <c r="C106" s="6" t="inlineStr">
+        <is>
+          <t>176scndcyc</t>
+        </is>
+      </c>
+      <c r="D106" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E106" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F106" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G106" s="6" t="n">
+        <v>4.34</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="6" t="inlineStr">
+        <is>
+          <t>2023-04-20</t>
+        </is>
+      </c>
+      <c r="B107" s="12" t="n">
+        <v>45036.40526238426</v>
+      </c>
+      <c r="C107" s="6" t="inlineStr">
+        <is>
+          <t>176fnlruntest</t>
+        </is>
+      </c>
+      <c r="D107" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E107" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F107" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G107" s="6" t="n">
+        <v>4.43</v>
       </c>
     </row>
     <row r="1048574" ht="12.8" customHeight="1" s="7"/>
@@ -3372,7 +3426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
@@ -4372,6 +4426,33 @@
         <v>4.52</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>2023-04-20</t>
+        </is>
+      </c>
+      <c r="B37" s="12" t="n">
+        <v>45036.50866017361</v>
+      </c>
+      <c r="C37" s="6" t="inlineStr">
+        <is>
+          <t>176beta</t>
+        </is>
+      </c>
+      <c r="D37" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E37" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F37" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" s="6" t="n">
+        <v>3.84</v>
+      </c>
+    </row>
     <row r="1048576" ht="15" customHeight="1" s="7"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -4386,7 +4467,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
@@ -6464,6 +6545,60 @@
       </c>
       <c r="G76" s="6" t="n">
         <v>4.04</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="6" t="inlineStr">
+        <is>
+          <t>2023-05-03</t>
+        </is>
+      </c>
+      <c r="B77" s="12" t="n">
+        <v>45049.6852472338</v>
+      </c>
+      <c r="C77" s="6" t="inlineStr">
+        <is>
+          <t>176firstsycle</t>
+        </is>
+      </c>
+      <c r="D77" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E77" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F77" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G77" s="6" t="n">
+        <v>4.18</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2023-05-08</t>
+        </is>
+      </c>
+      <c r="B78" s="12" t="n">
+        <v>45054.5333169482</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>176htfxtrl</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>269</v>
+      </c>
+      <c r="E78" t="n">
+        <v>266</v>
+      </c>
+      <c r="F78" t="n">
+        <v>3</v>
+      </c>
+      <c r="G78" t="n">
+        <v>4.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New UI changes in Candidate Lobby
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
@@ -3408,6 +3408,114 @@
       </c>
       <c r="G107" s="6" t="n">
         <v>4.43</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="6" t="inlineStr">
+        <is>
+          <t>2023-05-09</t>
+        </is>
+      </c>
+      <c r="B108" s="12" t="n">
+        <v>45055.67239</v>
+      </c>
+      <c r="C108" s="6" t="inlineStr">
+        <is>
+          <t>176htfxchanges</t>
+        </is>
+      </c>
+      <c r="D108" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E108" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F108" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G108" s="6" t="n">
+        <v>4.38</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="6" t="inlineStr">
+        <is>
+          <t>2023-05-09</t>
+        </is>
+      </c>
+      <c r="B109" s="12" t="n">
+        <v>45055.69151628472</v>
+      </c>
+      <c r="C109" s="6" t="inlineStr">
+        <is>
+          <t>176scndhtfx</t>
+        </is>
+      </c>
+      <c r="D109" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E109" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F109" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G109" s="6" t="n">
+        <v>4.84</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="6" t="inlineStr">
+        <is>
+          <t>2023-05-11</t>
+        </is>
+      </c>
+      <c r="B110" s="12" t="n">
+        <v>45057.72868366898</v>
+      </c>
+      <c r="C110" s="6" t="inlineStr">
+        <is>
+          <t>176fxhh</t>
+        </is>
+      </c>
+      <c r="D110" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E110" s="6" t="n">
+        <v>265</v>
+      </c>
+      <c r="F110" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G110" s="6" t="n">
+        <v>5.17</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2023-05-12</t>
+        </is>
+      </c>
+      <c r="B111" s="12" t="n">
+        <v>45058.76151206988</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>177fstcycle</t>
+        </is>
+      </c>
+      <c r="D111" t="n">
+        <v>269</v>
+      </c>
+      <c r="E111" t="n">
+        <v>263</v>
+      </c>
+      <c r="F111" t="n">
+        <v>6</v>
+      </c>
+      <c r="G111" t="n">
+        <v>7.72</v>
       </c>
     </row>
     <row r="1048574" ht="12.8" customHeight="1" s="7"/>
@@ -6575,29 +6683,29 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
+      <c r="A78" s="6" t="inlineStr">
         <is>
           <t>2023-05-08</t>
         </is>
       </c>
       <c r="B78" s="12" t="n">
-        <v>45054.5333169482</v>
-      </c>
-      <c r="C78" t="inlineStr">
+        <v>45054.53331694444</v>
+      </c>
+      <c r="C78" s="6" t="inlineStr">
         <is>
           <t>176htfxtrl</t>
         </is>
       </c>
-      <c r="D78" t="n">
-        <v>269</v>
-      </c>
-      <c r="E78" t="n">
+      <c r="D78" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E78" s="6" t="n">
         <v>266</v>
       </c>
-      <c r="F78" t="n">
+      <c r="F78" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="G78" t="n">
+      <c r="G78" s="6" t="n">
         <v>4.49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug Fixes in local attachments with ignore file
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMSIN" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BETA" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AMS" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="INDIA" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="AMSIN" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="BETA" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="AMS" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="INDIA" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G120"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
@@ -3735,30 +3735,84 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="inlineStr">
+      <c r="A120" s="6" t="inlineStr">
         <is>
           <t>2023-06-12</t>
         </is>
       </c>
       <c r="B120" s="12" t="n">
-        <v>45089.67016552043</v>
-      </c>
-      <c r="C120" t="inlineStr">
+        <v>45089.67016552083</v>
+      </c>
+      <c r="C120" s="6" t="inlineStr">
         <is>
           <t>178daytest</t>
         </is>
       </c>
-      <c r="D120" t="n">
-        <v>269</v>
-      </c>
-      <c r="E120" t="n">
+      <c r="D120" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E120" s="6" t="n">
         <v>264</v>
       </c>
-      <c r="F120" t="n">
+      <c r="F120" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="G120" t="n">
+      <c r="G120" s="6" t="n">
         <v>6.06</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="6" t="inlineStr">
+        <is>
+          <t>2023-07-31</t>
+        </is>
+      </c>
+      <c r="B121" s="12" t="n">
+        <v>45138.37467510417</v>
+      </c>
+      <c r="C121" s="6" t="inlineStr">
+        <is>
+          <t>180lastrun</t>
+        </is>
+      </c>
+      <c r="D121" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E121" s="6" t="n">
+        <v>262</v>
+      </c>
+      <c r="F121" s="6" t="n">
+        <v>7</v>
+      </c>
+      <c r="G121" s="6" t="n">
+        <v>6.52</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="6" t="inlineStr">
+        <is>
+          <t>2023-07-31</t>
+        </is>
+      </c>
+      <c r="B122" s="12" t="n">
+        <v>45138.3927577662</v>
+      </c>
+      <c r="C122" s="6" t="inlineStr">
+        <is>
+          <t>180fnlrun</t>
+        </is>
+      </c>
+      <c r="D122" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E122" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F122" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G122" s="6" t="n">
+        <v>4.04</v>
       </c>
     </row>
     <row r="1048574" ht="12.8" customHeight="1" s="7"/>
@@ -3777,7 +3831,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
@@ -4831,6 +4885,33 @@
         <v>4.39</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" s="6" t="inlineStr">
+        <is>
+          <t>2023-08-01</t>
+        </is>
+      </c>
+      <c r="B39" s="12" t="n">
+        <v>45139.52310601852</v>
+      </c>
+      <c r="C39" s="6" t="inlineStr">
+        <is>
+          <t>180beta</t>
+        </is>
+      </c>
+      <c r="D39" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E39" s="6" t="n">
+        <v>259</v>
+      </c>
+      <c r="F39" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G39" s="6" t="n">
+        <v>8.220000000000001</v>
+      </c>
+    </row>
     <row r="1048576" ht="15" customHeight="1" s="7"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -4845,7 +4926,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
@@ -7058,6 +7139,87 @@
       </c>
       <c r="G81" s="6" t="n">
         <v>3.81</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="6" t="inlineStr">
+        <is>
+          <t>2023-07-18</t>
+        </is>
+      </c>
+      <c r="B82" s="12" t="n">
+        <v>45125.7645241088</v>
+      </c>
+      <c r="C82" s="6" t="inlineStr">
+        <is>
+          <t>179htfxslots</t>
+        </is>
+      </c>
+      <c r="D82" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E82" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F82" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G82" s="6" t="n">
+        <v>3.77</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="6" t="inlineStr">
+        <is>
+          <t>2023-07-31</t>
+        </is>
+      </c>
+      <c r="B83" s="12" t="n">
+        <v>45138.81799356481</v>
+      </c>
+      <c r="C83" s="6" t="inlineStr">
+        <is>
+          <t>179scndhtfx</t>
+        </is>
+      </c>
+      <c r="D83" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E83" s="6" t="n">
+        <v>266</v>
+      </c>
+      <c r="F83" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G83" s="6" t="n">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2023-08-01</t>
+        </is>
+      </c>
+      <c r="B84" s="12" t="n">
+        <v>45139.83888939953</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>180live</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>269</v>
+      </c>
+      <c r="E84" t="n">
+        <v>265</v>
+      </c>
+      <c r="F84" t="n">
+        <v>4</v>
+      </c>
+      <c r="G84" t="n">
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix in 191
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G143"/>
+  <dimension ref="A1:G152"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
@@ -4356,30 +4356,273 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" t="inlineStr">
+      <c r="A143" s="6" t="inlineStr">
         <is>
           <t>2024-03-14</t>
         </is>
       </c>
       <c r="B143" s="12" t="n">
-        <v>45365.55358833045</v>
-      </c>
-      <c r="C143" t="inlineStr">
+        <v>45365.55358833334</v>
+      </c>
+      <c r="C143" s="6" t="inlineStr">
         <is>
           <t>189retest</t>
         </is>
       </c>
-      <c r="D143" t="n">
-        <v>269</v>
-      </c>
-      <c r="E143" t="n">
-        <v>269</v>
-      </c>
-      <c r="F143" t="n">
-        <v>0</v>
-      </c>
-      <c r="G143" t="n">
+      <c r="D143" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E143" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F143" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G143" s="6" t="n">
         <v>4.51</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="6" t="inlineStr">
+        <is>
+          <t>2024-03-28</t>
+        </is>
+      </c>
+      <c r="B144" s="12" t="n">
+        <v>45379.50678019676</v>
+      </c>
+      <c r="C144" s="6" t="inlineStr">
+        <is>
+          <t>190masstrail</t>
+        </is>
+      </c>
+      <c r="D144" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E144" s="6" t="n">
+        <v>266</v>
+      </c>
+      <c r="F144" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G144" s="6" t="n">
+        <v>5.21</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="6" t="inlineStr">
+        <is>
+          <t>2024-03-28</t>
+        </is>
+      </c>
+      <c r="B145" s="12" t="n">
+        <v>45379.67118087963</v>
+      </c>
+      <c r="C145" s="6" t="inlineStr">
+        <is>
+          <t>190fstcycle</t>
+        </is>
+      </c>
+      <c r="D145" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E145" s="6" t="n">
+        <v>268</v>
+      </c>
+      <c r="F145" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G145" s="6" t="n">
+        <v>5.21</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="6" t="inlineStr">
+        <is>
+          <t>2024-03-29</t>
+        </is>
+      </c>
+      <c r="B146" s="12" t="n">
+        <v>45380.45194586806</v>
+      </c>
+      <c r="C146" s="6" t="inlineStr">
+        <is>
+          <t>190scndcycle</t>
+        </is>
+      </c>
+      <c r="D146" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E146" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F146" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G146" s="6" t="n">
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="6" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="B147" s="12" t="n">
+        <v>45383.37318597222</v>
+      </c>
+      <c r="C147" s="6" t="inlineStr">
+        <is>
+          <t>190fnlrun</t>
+        </is>
+      </c>
+      <c r="D147" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E147" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F147" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G147" s="6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="6" t="inlineStr">
+        <is>
+          <t>2024-04-25</t>
+        </is>
+      </c>
+      <c r="B148" s="12" t="n">
+        <v>45407.45201841435</v>
+      </c>
+      <c r="C148" s="6" t="inlineStr">
+        <is>
+          <t>191trail</t>
+        </is>
+      </c>
+      <c r="D148" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E148" s="6" t="n">
+        <v>266</v>
+      </c>
+      <c r="F148" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G148" s="6" t="n">
+        <v>5.18</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="6" t="inlineStr">
+        <is>
+          <t>2024-05-02</t>
+        </is>
+      </c>
+      <c r="B149" s="12" t="n">
+        <v>45414.48380873843</v>
+      </c>
+      <c r="C149" s="6" t="inlineStr">
+        <is>
+          <t>191fstcycle</t>
+        </is>
+      </c>
+      <c r="D149" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E149" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F149" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G149" s="6" t="n">
+        <v>4.51</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="6" t="inlineStr">
+        <is>
+          <t>2024-05-03</t>
+        </is>
+      </c>
+      <c r="B150" s="12" t="n">
+        <v>45415.3477190625</v>
+      </c>
+      <c r="C150" s="6" t="inlineStr">
+        <is>
+          <t>191lstrun</t>
+        </is>
+      </c>
+      <c r="D150" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E150" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F150" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G150" s="6" t="n">
+        <v>4.64</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="6" t="inlineStr">
+        <is>
+          <t>2024-05-06</t>
+        </is>
+      </c>
+      <c r="B151" s="12" t="n">
+        <v>45418.45908497685</v>
+      </c>
+      <c r="C151" s="6" t="inlineStr">
+        <is>
+          <t>sampletestevent12</t>
+        </is>
+      </c>
+      <c r="D151" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E151" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F151" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G151" s="6" t="n">
+        <v>4.13</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2024-05-06</t>
+        </is>
+      </c>
+      <c r="B152" s="12" t="n">
+        <v>45418.52041275083</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>191bugfix</t>
+        </is>
+      </c>
+      <c r="D152" t="n">
+        <v>269</v>
+      </c>
+      <c r="E152" t="n">
+        <v>269</v>
+      </c>
+      <c r="F152" t="n">
+        <v>0</v>
+      </c>
+      <c r="G152" t="n">
+        <v>4.34</v>
       </c>
     </row>
     <row r="1048574" ht="12.8" customHeight="1" s="7"/>
@@ -4398,7 +4641,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
@@ -5668,6 +5911,60 @@
         <v>6.27</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" s="6" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="B47" s="12" t="n">
+        <v>45383.53779894676</v>
+      </c>
+      <c r="C47" s="6" t="inlineStr">
+        <is>
+          <t>190betatest</t>
+        </is>
+      </c>
+      <c r="D47" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E47" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F47" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G47" s="6" t="n">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="6" t="inlineStr">
+        <is>
+          <t>2024-05-03</t>
+        </is>
+      </c>
+      <c r="B48" s="12" t="n">
+        <v>45415.60846070602</v>
+      </c>
+      <c r="C48" s="6" t="inlineStr">
+        <is>
+          <t>191beta</t>
+        </is>
+      </c>
+      <c r="D48" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E48" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F48" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" s="6" t="n">
+        <v>4.74</v>
+      </c>
+    </row>
     <row r="1048576" ht="15" customHeight="1" s="7"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -5682,7 +5979,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G99"/>
+  <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
@@ -8381,6 +8678,33 @@
       </c>
       <c r="G99" s="6" t="n">
         <v>7.22</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="6" t="inlineStr">
+        <is>
+          <t>2024-04-01</t>
+        </is>
+      </c>
+      <c r="B100" s="12" t="n">
+        <v>45383.85344318287</v>
+      </c>
+      <c r="C100" s="6" t="inlineStr">
+        <is>
+          <t>190livee</t>
+        </is>
+      </c>
+      <c r="D100" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E100" s="6" t="n">
+        <v>267</v>
+      </c>
+      <c r="F100" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G100" s="6" t="n">
+        <v>4.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Appicant Custom properties script
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/E2E_REGRESSION_HISTORY_DATA.xlsx
@@ -4599,29 +4599,29 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" t="inlineStr">
+      <c r="A152" s="6" t="inlineStr">
         <is>
           <t>2024-05-06</t>
         </is>
       </c>
       <c r="B152" s="12" t="n">
-        <v>45418.52041275083</v>
-      </c>
-      <c r="C152" t="inlineStr">
+        <v>45418.52041275463</v>
+      </c>
+      <c r="C152" s="6" t="inlineStr">
         <is>
           <t>191bugfix</t>
         </is>
       </c>
-      <c r="D152" t="n">
-        <v>269</v>
-      </c>
-      <c r="E152" t="n">
-        <v>269</v>
-      </c>
-      <c r="F152" t="n">
-        <v>0</v>
-      </c>
-      <c r="G152" t="n">
+      <c r="D152" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="E152" s="6" t="n">
+        <v>269</v>
+      </c>
+      <c r="F152" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G152" s="6" t="n">
         <v>4.34</v>
       </c>
     </row>
@@ -5979,7 +5979,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
@@ -8705,6 +8705,33 @@
       </c>
       <c r="G100" s="6" t="n">
         <v>4.89</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2024-05-06</t>
+        </is>
+      </c>
+      <c r="B101" s="12" t="n">
+        <v>45418.56465067549</v>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>191live</t>
+        </is>
+      </c>
+      <c r="D101" t="n">
+        <v>269</v>
+      </c>
+      <c r="E101" t="n">
+        <v>255</v>
+      </c>
+      <c r="F101" t="n">
+        <v>14</v>
+      </c>
+      <c r="G101" t="n">
+        <v>8.359999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>